<commit_message>
- updated Excel for performance data and graphs.
</commit_message>
<xml_diff>
--- a/PA3_Data.xlsx
+++ b/PA3_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tungh\Desktop\CS430\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE6EDBA-AFB3-4291-A454-C689FF1A88BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD153D99-F5B1-41B9-AD23-8D63C52ECD15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08165E98-1035-4888-9355-07EE148DA466}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{08165E98-1035-4888-9355-07EE148DA466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Threads</t>
   </si>
@@ -48,13 +48,25 @@
     <t>OpenMP, sec</t>
   </si>
   <si>
-    <t>Run Time Ratio</t>
-  </si>
-  <si>
     <t>p = N / Threads</t>
   </si>
   <si>
     <t>Speed Up</t>
+  </si>
+  <si>
+    <t>Run Time Ratio (OpenMP versus Serial)</t>
+  </si>
+  <si>
+    <t>Run Time Ratio (OpenMP versus OpenMP)</t>
+  </si>
+  <si>
+    <t>OpenMP, sec (single thread)</t>
+  </si>
+  <si>
+    <t>NOTES:</t>
+  </si>
+  <si>
+    <t>single-threaded OpenMP program already faster than default Linux single-threaded program. So, be careful about what timer to use in order to measure performance.</t>
   </si>
 </sst>
 </file>
@@ -70,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,6 +92,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,9 +114,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,88 +261,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>1.4E-5</c:v>
+                  <c:v>2.3E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8700000000000005E-4</c:v>
+                  <c:v>1.05E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.189E-3</c:v>
+                  <c:v>9.2999999999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.518E-3</c:v>
+                  <c:v>3.4E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.799E-3</c:v>
+                  <c:v>3.1000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1380000000000001E-3</c:v>
+                  <c:v>3.8000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4269999999999999E-3</c:v>
+                  <c:v>8.2999999999999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7629999999999998E-3</c:v>
+                  <c:v>3.1000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0400000000000002E-3</c:v>
+                  <c:v>8.8999999999999995E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2680000000000001E-3</c:v>
+                  <c:v>3.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.653E-3</c:v>
+                  <c:v>2.9E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.0049999999999999E-3</c:v>
+                  <c:v>3.3000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.3319999999999999E-3</c:v>
+                  <c:v>9.6000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.7200000000000002E-3</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.1130000000000004E-3</c:v>
+                  <c:v>3.6999999999999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.437E-3</c:v>
+                  <c:v>3.3000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.692E-3</c:v>
+                  <c:v>3.4E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.9930000000000001E-3</c:v>
+                  <c:v>3.1000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.2989999999999999E-3</c:v>
+                  <c:v>5.5999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.6680000000000003E-3</c:v>
+                  <c:v>3.8000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.9740000000000002E-3</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.3239999999999998E-3</c:v>
+                  <c:v>3.8999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.6429999999999996E-3</c:v>
+                  <c:v>3.4999999999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.038E-3</c:v>
+                  <c:v>3.4999999999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.3059999999999991E-3</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.7670000000000005E-3</c:v>
+                  <c:v>3.6000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.0830000000000008E-3</c:v>
+                  <c:v>4.1999999999999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.2635E-2</c:v>
+                  <c:v>4.6999999999999997E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -619,88 +644,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>3.7000000000000002E-3</c:v>
+                  <c:v>9.9819999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0829999999999999E-3</c:v>
+                  <c:v>4.9540000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8860000000000006E-3</c:v>
+                  <c:v>3.346E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2429999999999995E-3</c:v>
+                  <c:v>2.6329999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0352999999999999E-2</c:v>
+                  <c:v>2.14E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1417E-2</c:v>
+                  <c:v>1.8760000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2363000000000001E-2</c:v>
+                  <c:v>1.5299999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3112E-2</c:v>
+                  <c:v>1.426E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3971000000000001E-2</c:v>
+                  <c:v>1.3359999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4744999999999999E-2</c:v>
+                  <c:v>1.2080000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5446E-2</c:v>
+                  <c:v>1.103E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6191000000000001E-2</c:v>
+                  <c:v>1.0219999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.6803999999999999E-2</c:v>
+                  <c:v>9.5600000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.7451999999999999E-2</c:v>
+                  <c:v>8.8900000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.8022E-2</c:v>
+                  <c:v>8.3299999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.8637999999999998E-2</c:v>
+                  <c:v>8.2399999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.9231000000000002E-2</c:v>
+                  <c:v>7.27E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.9769999999999999E-2</c:v>
+                  <c:v>6.8499999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0338999999999999E-2</c:v>
+                  <c:v>7.1000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0763E-2</c:v>
+                  <c:v>6.7299999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1249000000000001E-2</c:v>
+                  <c:v>6.4499999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1651E-2</c:v>
+                  <c:v>5.62E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2155999999999999E-2</c:v>
+                  <c:v>5.8900000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2623000000000001E-2</c:v>
+                  <c:v>5.2800000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3146E-2</c:v>
+                  <c:v>5.5800000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.3569E-2</c:v>
+                  <c:v>4.7899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5309999999999999E-2</c:v>
+                  <c:v>5.3399999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.2970999999999997E-2</c:v>
+                  <c:v>5.1199999999999998E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -997,7 +1022,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$30</c:f>
+              <c:f>Sheet1!$N$3:$N$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
@@ -1380,7 +1405,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$33:$L$60</c:f>
+              <c:f>Sheet1!$N$33:$N$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
@@ -3876,13 +3901,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>21167</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>4234</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>10584</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>148166</xdr:rowOff>
@@ -3912,13 +3937,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>10582</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>21166</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>179916</xdr:rowOff>
@@ -3948,13 +3973,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>14816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>21167</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>169332</xdr:rowOff>
@@ -3984,13 +4009,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>21166</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>14816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>21166</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>148165</xdr:rowOff>
@@ -4318,10 +4343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35F2EC4-7841-4F22-821C-FC0DD5723D9B}">
-  <dimension ref="B2:L60"/>
+  <dimension ref="B2:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4332,19 +4357,21 @@
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" t="s">
@@ -4353,88 +4380,108 @@
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <f>C3/1000</f>
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="F3">
         <v>1000</v>
       </c>
       <c r="G3">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1.4E-5</v>
+        <v>2.3E-5</v>
       </c>
       <c r="J3">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K3" s="2">
         <f>G3/I3</f>
-        <v>285.71428571428572</v>
-      </c>
-      <c r="K3">
+        <v>130.43478260869566</v>
+      </c>
+      <c r="L3">
+        <f>J3/I3</f>
+        <v>1</v>
+      </c>
+      <c r="M3">
         <f>F3/H3/F3</f>
         <v>1</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2000</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D22" si="0">C4/1000</f>
-        <v>7.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F4">
         <v>1000</v>
       </c>
       <c r="G4">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4">
-        <v>7.8700000000000005E-4</v>
+        <v>1.05E-4</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J30" si="1">G4/I4</f>
-        <v>5.082592121982211</v>
+        <v>2.3E-5</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K60" si="2">F4/H4/F4</f>
+        <f t="shared" ref="K4:K30" si="1">G4/I4</f>
+        <v>28.571428571428569</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L30" si="2">J4/I4</f>
+        <v>0.21904761904761905</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M60" si="3">F4/H4/F4</f>
         <v>0.5</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L60" si="3">1/(1-K4+K4/F4)</f>
+      <c r="N4">
+        <f t="shared" ref="N4:N60" si="4">1/(1-M4+M4/F4)</f>
         <v>1.9980019980019983</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3000</v>
       </c>
@@ -4449,100 +4496,121 @@
         <v>1000</v>
       </c>
       <c r="G5">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5">
-        <v>1.189E-3</v>
+        <v>9.2999999999999997E-5</v>
       </c>
       <c r="J5">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="1"/>
-        <v>3.3641715727502106</v>
-      </c>
-      <c r="K5">
+        <v>32.258064516129032</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="2"/>
+        <v>0.24731182795698925</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L5">
-        <f t="shared" si="3"/>
+      <c r="N5">
+        <f t="shared" si="4"/>
         <v>1.4992503748125936</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4000</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1.2999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F6">
         <v>1000</v>
       </c>
       <c r="G6">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H6">
         <v>4</v>
       </c>
       <c r="I6">
-        <v>1.518E-3</v>
+        <v>3.4E-5</v>
       </c>
       <c r="J6">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="1"/>
-        <v>2.6350461133069829</v>
-      </c>
-      <c r="K6">
+        <v>88.235294117647058</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="2"/>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="3"/>
+      <c r="N6">
+        <f t="shared" si="4"/>
         <v>1.3328890369876709</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F7">
         <v>1000</v>
       </c>
       <c r="G7">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H7">
         <v>5</v>
       </c>
       <c r="I7">
-        <v>1.799E-3</v>
+        <v>3.1000000000000001E-5</v>
       </c>
       <c r="J7">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="1"/>
-        <v>2.2234574763757644</v>
-      </c>
-      <c r="K7">
+        <v>96.774193548387089</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="2"/>
+        <v>0.74193548387096775</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="L7">
-        <f t="shared" si="3"/>
+      <c r="N7">
+        <f t="shared" si="4"/>
         <v>1.2496875781054737</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>10000</v>
       </c>
@@ -4557,741 +4625,930 @@
         <v>1000</v>
       </c>
       <c r="G8">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H8">
         <v>6</v>
       </c>
       <c r="I8">
-        <v>2.1380000000000001E-3</v>
+        <v>3.8000000000000002E-5</v>
       </c>
       <c r="J8">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="1"/>
-        <v>1.8709073900841908</v>
-      </c>
-      <c r="K8">
+        <v>78.94736842105263</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="2"/>
+        <v>0.60526315789473684</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="L8">
-        <f t="shared" si="3"/>
+      <c r="N8">
+        <f t="shared" si="4"/>
         <v>1.1997600479904018</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>20000</v>
       </c>
       <c r="C9">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F9">
         <v>1000</v>
       </c>
       <c r="G9">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H9">
         <v>7</v>
       </c>
       <c r="I9">
-        <v>2.4269999999999999E-3</v>
+        <v>8.2999999999999998E-5</v>
       </c>
       <c r="J9">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="1"/>
-        <v>1.6481252575195715</v>
-      </c>
-      <c r="K9">
+        <v>36.144578313253014</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="2"/>
+        <v>0.27710843373493976</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="L9">
-        <f t="shared" si="3"/>
+      <c r="N9">
+        <f t="shared" si="4"/>
         <v>1.1664722546242292</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>30000</v>
       </c>
       <c r="C10">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.104</v>
+        <v>0.105</v>
       </c>
       <c r="F10">
         <v>1000</v>
       </c>
       <c r="G10">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H10">
         <v>8</v>
       </c>
       <c r="I10">
-        <v>2.7629999999999998E-3</v>
+        <v>3.1000000000000001E-5</v>
       </c>
       <c r="J10">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="1"/>
-        <v>1.4477017734346727</v>
-      </c>
-      <c r="K10">
+        <v>96.774193548387089</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="2"/>
+        <v>0.74193548387096775</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
-      <c r="L10">
-        <f t="shared" si="3"/>
+      <c r="N10">
+        <f t="shared" si="4"/>
         <v>1.142693900871304</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>40000</v>
       </c>
       <c r="C11">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="F11">
         <v>1000</v>
       </c>
       <c r="G11">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H11">
         <v>9</v>
       </c>
       <c r="I11">
-        <v>3.0400000000000002E-3</v>
+        <v>8.8999999999999995E-5</v>
       </c>
       <c r="J11">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="1"/>
-        <v>1.3157894736842104</v>
-      </c>
-      <c r="K11">
+        <v>33.707865168539328</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="2"/>
+        <v>0.25842696629213485</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
         <v>0.11111111111111112</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="3"/>
+      <c r="N11">
+        <f t="shared" si="4"/>
         <v>1.124859392575928</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>50000</v>
       </c>
       <c r="C12">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0.182</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="F12">
         <v>1000</v>
       </c>
       <c r="G12">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H12">
         <v>10</v>
       </c>
       <c r="I12">
-        <v>3.2680000000000001E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="J12">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="1"/>
-        <v>1.2239902080783354</v>
-      </c>
-      <c r="K12">
+        <v>100</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="2"/>
+        <v>0.76666666666666661</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="3"/>
+      <c r="N12">
+        <f t="shared" si="4"/>
         <v>1.1109876680368849</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>100000</v>
       </c>
       <c r="C13">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0.34699999999999998</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="F13">
         <v>1000</v>
       </c>
       <c r="G13">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H13">
         <v>11</v>
       </c>
       <c r="I13">
-        <v>3.653E-3</v>
+        <v>2.9E-5</v>
       </c>
       <c r="J13">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="1"/>
-        <v>1.0949904188338353</v>
-      </c>
-      <c r="K13">
+        <v>103.44827586206897</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="2"/>
+        <v>0.7931034482758621</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
+      <c r="N13">
+        <f t="shared" si="4"/>
         <v>1.0998900109989</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>200000</v>
       </c>
       <c r="C14">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>0.70299999999999996</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="F14">
         <v>1000</v>
       </c>
       <c r="G14">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H14">
         <v>12</v>
       </c>
       <c r="I14">
-        <v>4.0049999999999999E-3</v>
+        <v>3.3000000000000003E-5</v>
       </c>
       <c r="J14">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="1"/>
-        <v>0.99875156054931336</v>
-      </c>
-      <c r="K14">
+        <v>90.909090909090907</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="2"/>
+        <v>0.69696969696969691</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="3"/>
+      <c r="N14">
+        <f t="shared" si="4"/>
         <v>1.0908099263703299</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>300000</v>
       </c>
       <c r="C15">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1.056</v>
+        <v>1.052</v>
       </c>
       <c r="F15">
         <v>1000</v>
       </c>
       <c r="G15">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H15">
         <v>13</v>
       </c>
       <c r="I15">
-        <v>4.3319999999999999E-3</v>
+        <v>9.6000000000000002E-5</v>
       </c>
       <c r="J15">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="1"/>
-        <v>0.92336103416435833</v>
-      </c>
-      <c r="K15">
+        <v>31.25</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="2"/>
+        <v>0.23958333333333331</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
         <v>7.6923076923076913E-2</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="3"/>
+      <c r="N15">
+        <f t="shared" si="4"/>
         <v>1.0832430630780767</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>400000</v>
       </c>
       <c r="C16">
-        <v>1302</v>
+        <v>1396</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1.302</v>
+        <v>1.3959999999999999</v>
       </c>
       <c r="F16">
         <v>1000</v>
       </c>
       <c r="G16">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H16">
         <v>14</v>
       </c>
       <c r="I16">
-        <v>4.7200000000000002E-3</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="J16">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="1"/>
-        <v>0.84745762711864403</v>
-      </c>
-      <c r="K16">
+        <v>75</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="2"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="3"/>
+      <c r="N16">
+        <f t="shared" si="4"/>
         <v>1.0768402430582262</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>500000</v>
       </c>
       <c r="C17">
-        <v>1561</v>
+        <v>1741</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1.5609999999999999</v>
+        <v>1.7410000000000001</v>
       </c>
       <c r="F17">
         <v>1000</v>
       </c>
       <c r="G17">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H17">
         <v>15</v>
       </c>
       <c r="I17">
-        <v>5.1130000000000004E-3</v>
+        <v>3.6999999999999998E-5</v>
       </c>
       <c r="J17">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="1"/>
-        <v>0.78231957754742809</v>
-      </c>
-      <c r="K17">
+        <v>81.081081081081081</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="2"/>
+        <v>0.6216216216216216</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="3"/>
+      <c r="N17">
+        <f t="shared" si="4"/>
         <v>1.0713520462824084</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
         <v>1000000</v>
       </c>
       <c r="C18">
-        <v>3508</v>
+        <v>3489</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="F18">
         <v>1000</v>
       </c>
       <c r="G18">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H18">
         <v>16</v>
       </c>
       <c r="I18">
-        <v>5.437E-3</v>
+        <v>3.3000000000000003E-5</v>
       </c>
       <c r="J18">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="1"/>
-        <v>0.73569983446753728</v>
-      </c>
-      <c r="K18">
+        <v>90.909090909090907</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="2"/>
+        <v>0.69696969696969691</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
         <v>6.25E-2</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="3"/>
+      <c r="N18">
+        <f t="shared" si="4"/>
         <v>1.0665955602959802</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2000000</v>
       </c>
       <c r="C19">
-        <v>6661</v>
+        <v>6451</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>6.6609999999999996</v>
+        <v>6.4509999999999996</v>
       </c>
       <c r="F19">
         <v>1000</v>
       </c>
       <c r="G19">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H19">
         <v>17</v>
       </c>
       <c r="I19">
-        <v>5.692E-3</v>
+        <v>3.4E-5</v>
       </c>
       <c r="J19">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="1"/>
-        <v>0.70274068868587491</v>
-      </c>
-      <c r="K19">
+        <v>88.235294117647058</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="2"/>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="3"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="3"/>
+      <c r="N19">
+        <f t="shared" si="4"/>
         <v>1.0624335979001311</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>3000000</v>
       </c>
       <c r="C20">
-        <v>8631</v>
+        <v>9097</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>8.6310000000000002</v>
+        <v>9.0969999999999995</v>
       </c>
       <c r="F20">
         <v>1000</v>
       </c>
       <c r="G20">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H20">
         <v>18</v>
       </c>
       <c r="I20">
-        <v>5.9930000000000001E-3</v>
+        <v>3.1000000000000001E-5</v>
       </c>
       <c r="J20">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="1"/>
-        <v>0.66744535291173035</v>
-      </c>
-      <c r="K20">
+        <v>96.774193548387089</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="2"/>
+        <v>0.74193548387096775</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
         <v>5.5555555555555559E-2</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="3"/>
+      <c r="N20">
+        <f t="shared" si="4"/>
         <v>1.0587612493382743</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>4000000</v>
       </c>
       <c r="C21">
-        <v>11344</v>
+        <v>11374</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>11.343999999999999</v>
+        <v>11.374000000000001</v>
       </c>
       <c r="F21">
         <v>1000</v>
       </c>
       <c r="G21">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H21">
         <v>19</v>
       </c>
       <c r="I21">
-        <v>6.2989999999999999E-3</v>
+        <v>5.5999999999999999E-5</v>
       </c>
       <c r="J21">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="1"/>
-        <v>0.63502143197332916</v>
-      </c>
-      <c r="K21">
+        <v>53.571428571428577</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="2"/>
+        <v>0.4107142857142857</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
         <v>5.2631578947368418E-2</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="3"/>
+      <c r="N21">
+        <f t="shared" si="4"/>
         <v>1.0554969168379533</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>5000000</v>
       </c>
       <c r="C22">
-        <v>14156</v>
+        <v>14778</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>14.156000000000001</v>
+        <v>14.778</v>
       </c>
       <c r="F22">
         <v>1000</v>
       </c>
       <c r="G22">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H22">
         <v>20</v>
       </c>
       <c r="I22">
-        <v>6.6680000000000003E-3</v>
+        <v>3.8000000000000002E-5</v>
       </c>
       <c r="J22">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="1"/>
-        <v>0.59988002399520091</v>
-      </c>
-      <c r="K22">
+        <v>78.94736842105263</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="2"/>
+        <v>0.60526315789473684</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="L22">
-        <f t="shared" si="3"/>
+      <c r="N22">
+        <f t="shared" si="4"/>
         <v>1.052576180201042</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>1000</v>
       </c>
       <c r="G23">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H23">
         <v>21</v>
       </c>
       <c r="I23">
-        <v>6.9740000000000002E-3</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="J23">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="1"/>
-        <v>0.57355893318038431</v>
-      </c>
-      <c r="K23">
+        <v>75</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="2"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
         <v>4.7619047619047623E-2</v>
       </c>
-      <c r="L23">
-        <f t="shared" si="3"/>
+      <c r="N23">
+        <f t="shared" si="4"/>
         <v>1.0499475026248688</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F24">
         <v>1000</v>
       </c>
       <c r="G24">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H24">
         <v>22</v>
       </c>
       <c r="I24">
-        <v>7.3239999999999998E-3</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="J24">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="1"/>
-        <v>0.54614964500273078</v>
-      </c>
-      <c r="K24">
+        <v>76.92307692307692</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="2"/>
+        <v>0.58974358974358976</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="L24">
-        <f t="shared" si="3"/>
+      <c r="N24">
+        <f t="shared" si="4"/>
         <v>1.0475691633731727</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
       <c r="F25">
         <v>1000</v>
       </c>
       <c r="G25">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H25">
         <v>23</v>
       </c>
       <c r="I25">
-        <v>7.6429999999999996E-3</v>
+        <v>3.4999999999999997E-5</v>
       </c>
       <c r="J25">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="1"/>
-        <v>0.52335470365039904</v>
-      </c>
-      <c r="K25">
+        <v>85.714285714285722</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="2"/>
+        <v>0.65714285714285725</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="L25">
-        <f t="shared" si="3"/>
+      <c r="N25">
+        <f t="shared" si="4"/>
         <v>1.0454070269533202</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
       <c r="F26">
         <v>1000</v>
       </c>
       <c r="G26">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H26">
         <v>24</v>
       </c>
       <c r="I26">
-        <v>8.038E-3</v>
+        <v>3.4999999999999997E-5</v>
       </c>
       <c r="J26">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="1"/>
-        <v>0.49763622791739237</v>
-      </c>
-      <c r="K26">
+        <v>85.714285714285722</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="2"/>
+        <v>0.65714285714285725</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="3"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="L26">
-        <f t="shared" si="3"/>
+      <c r="N26">
+        <f t="shared" si="4"/>
         <v>1.0434328942219901</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="F27">
         <v>1000</v>
       </c>
       <c r="G27">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H27">
         <v>25</v>
       </c>
       <c r="I27">
-        <v>8.3059999999999991E-3</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="J27">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="1"/>
-        <v>0.48157958102576459</v>
-      </c>
-      <c r="K27">
+        <v>75</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="2"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
-      <c r="L27">
-        <f t="shared" si="3"/>
+      <c r="N27">
+        <f t="shared" si="4"/>
         <v>1.0416232656972626</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
       <c r="F28">
         <v>1000</v>
       </c>
       <c r="G28">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H28">
         <v>26</v>
       </c>
       <c r="I28">
-        <v>8.7670000000000005E-3</v>
+        <v>3.6000000000000001E-5</v>
       </c>
       <c r="J28">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="1"/>
-        <v>0.45625641610585149</v>
-      </c>
-      <c r="K28">
+        <v>83.333333333333329</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="2"/>
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="3"/>
         <v>3.8461538461538457E-2</v>
       </c>
-      <c r="L28">
-        <f t="shared" si="3"/>
+      <c r="N28">
+        <f t="shared" si="4"/>
         <v>1.0399584016639334</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
       <c r="F29">
         <v>1000</v>
       </c>
       <c r="G29">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H29">
         <v>27</v>
       </c>
       <c r="I29">
-        <v>9.0830000000000008E-3</v>
+        <v>4.1999999999999998E-5</v>
       </c>
       <c r="J29">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="1"/>
-        <v>0.4403831333259936</v>
-      </c>
-      <c r="K29">
+        <v>71.428571428571431</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="2"/>
+        <v>0.54761904761904767</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="3"/>
         <v>3.7037037037037035E-2</v>
       </c>
-      <c r="L29">
-        <f t="shared" si="3"/>
+      <c r="N29">
+        <f t="shared" si="4"/>
         <v>1.0384215991692627</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
       <c r="F30">
         <v>1000</v>
       </c>
       <c r="G30">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H30">
         <v>28</v>
       </c>
       <c r="I30">
-        <v>1.2635E-2</v>
+        <v>4.6999999999999997E-5</v>
       </c>
       <c r="J30">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="1"/>
-        <v>0.31658092599920856</v>
-      </c>
-      <c r="K30">
+        <v>63.829787234042556</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="2"/>
+        <v>0.48936170212765961</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="3"/>
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="L30">
-        <f t="shared" si="3"/>
+      <c r="N30">
+        <f t="shared" si="4"/>
         <v>1.0369986296803821</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G32" t="s">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H32" t="s">
@@ -5300,745 +5557,955 @@
       <c r="I32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K32" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" t="s">
         <v>4</v>
       </c>
-      <c r="K32" t="s">
+      <c r="N32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F33">
         <v>1000000</v>
       </c>
       <c r="G33">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
-        <v>3.7000000000000002E-3</v>
+        <v>9.9819999999999996E-3</v>
       </c>
       <c r="J33">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K33" s="2">
         <f>G33/I33</f>
-        <v>948.10810810810801</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="2"/>
+        <v>349.52915247445401</v>
+      </c>
+      <c r="L33">
+        <f>J33/I33</f>
         <v>1</v>
       </c>
-      <c r="L33">
+      <c r="M33">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F34">
         <v>1000000</v>
       </c>
       <c r="G34">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H34">
         <v>2</v>
       </c>
       <c r="I34">
-        <v>6.0829999999999999E-3</v>
+        <v>4.9540000000000001E-3</v>
       </c>
       <c r="J34">
-        <f t="shared" ref="J34:J60" si="4">G34/I34</f>
-        <v>576.68913365115895</v>
+        <v>9.9819999999999996E-3</v>
       </c>
       <c r="K34">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K34:K60" si="5">G34/I34</f>
+        <v>704.27937020589422</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ref="L34:L60" si="6">J34/I34</f>
+        <v>2.0149374243035929</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="L34">
-        <f t="shared" si="3"/>
+      <c r="N34">
+        <f t="shared" si="4"/>
         <v>1.9999980000020001</v>
       </c>
     </row>
-    <row r="35" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F35">
         <v>1000000</v>
       </c>
       <c r="G35">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H35">
         <v>3</v>
       </c>
       <c r="I35">
-        <v>7.8860000000000006E-3</v>
+        <v>3.346E-3</v>
       </c>
       <c r="J35">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="5"/>
+        <v>1042.7375971309025</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="6"/>
+        <v>2.9832635983263596</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N35">
         <f t="shared" si="4"/>
-        <v>444.83895511032205</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="3"/>
         <v>1.4999992500003747</v>
       </c>
     </row>
-    <row r="36" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F36">
         <v>1000000</v>
       </c>
       <c r="G36">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H36">
         <v>4</v>
       </c>
       <c r="I36">
-        <v>9.2429999999999995E-3</v>
+        <v>2.6329999999999999E-3</v>
       </c>
       <c r="J36">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="5"/>
+        <v>1325.1044436004559</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="6"/>
+        <v>3.7911127990884923</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="N36">
         <f t="shared" si="4"/>
-        <v>379.53045547982259</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="3"/>
         <v>1.333332888889037</v>
       </c>
     </row>
-    <row r="37" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F37">
         <v>1000000</v>
       </c>
       <c r="G37">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H37">
         <v>5</v>
       </c>
       <c r="I37">
-        <v>1.0352999999999999E-2</v>
+        <v>2.14E-3</v>
       </c>
       <c r="J37">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="5"/>
+        <v>1630.3738317757009</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="6"/>
+        <v>4.6644859813084114</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="N37">
         <f t="shared" si="4"/>
-        <v>338.83898386940984</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="3"/>
         <v>1.2499996875000781</v>
       </c>
     </row>
-    <row r="38" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F38">
         <v>1000000</v>
       </c>
       <c r="G38">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H38">
         <v>6</v>
       </c>
       <c r="I38">
-        <v>1.1417E-2</v>
+        <v>1.8760000000000001E-3</v>
       </c>
       <c r="J38">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="5"/>
+        <v>1859.8081023454156</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="6"/>
+        <v>5.3208955223880592</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N38">
         <f t="shared" si="4"/>
-        <v>307.26110186563898</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="3"/>
         <v>1.1999997600000478</v>
       </c>
     </row>
-    <row r="39" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F39">
         <v>1000000</v>
       </c>
       <c r="G39">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H39">
         <v>7</v>
       </c>
       <c r="I39">
-        <v>1.2363000000000001E-2</v>
+        <v>1.5299999999999999E-3</v>
       </c>
       <c r="J39">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="5"/>
+        <v>2280.3921568627452</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="6"/>
+        <v>6.5241830065359476</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="3"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="N39">
         <f t="shared" si="4"/>
-        <v>283.74989889185468</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="2"/>
-        <v>0.14285714285714288</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="3"/>
         <v>1.1666664722222546</v>
       </c>
     </row>
-    <row r="40" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F40">
         <v>1000000</v>
       </c>
       <c r="G40">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H40">
         <v>8</v>
       </c>
       <c r="I40">
-        <v>1.3112E-2</v>
+        <v>1.426E-3</v>
       </c>
       <c r="J40">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="5"/>
+        <v>2446.7040673211782</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+      <c r="N40">
         <f t="shared" si="4"/>
-        <v>267.54118364856618</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="2"/>
-        <v>0.125</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="3"/>
         <v>1.1428569795918599</v>
       </c>
     </row>
-    <row r="41" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F41">
         <v>1000000</v>
       </c>
       <c r="G41">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H41">
         <v>9</v>
       </c>
       <c r="I41">
-        <v>1.3971000000000001E-2</v>
+        <v>1.3359999999999999E-3</v>
       </c>
       <c r="J41">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="5"/>
+        <v>2611.5269461077846</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="6"/>
+        <v>7.4715568862275452</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="3"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="N41">
         <f t="shared" si="4"/>
-        <v>251.09154677546346</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="3"/>
         <v>1.1249998593750177</v>
       </c>
     </row>
-    <row r="42" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F42">
         <v>1000000</v>
       </c>
       <c r="G42">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H42">
         <v>10</v>
       </c>
       <c r="I42">
-        <v>1.4744999999999999E-2</v>
+        <v>1.2080000000000001E-3</v>
       </c>
       <c r="J42">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="5"/>
+        <v>2888.2450331125824</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="6"/>
+        <v>8.2632450331125824</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="N42">
         <f t="shared" si="4"/>
-        <v>237.91115632417771</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="3"/>
         <v>1.1111109876543348</v>
       </c>
     </row>
-    <row r="43" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F43">
         <v>1000000</v>
       </c>
       <c r="G43">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H43">
         <v>11</v>
       </c>
       <c r="I43">
-        <v>1.5446E-2</v>
+        <v>1.103E-3</v>
       </c>
       <c r="J43">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="5"/>
+        <v>3163.1912964641883</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="6"/>
+        <v>9.0498640072529462</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="3"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="N43">
         <f t="shared" si="4"/>
-        <v>227.11381587466011</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="3"/>
         <v>1.099999890000011</v>
       </c>
     </row>
-    <row r="44" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F44">
         <v>1000000</v>
       </c>
       <c r="G44">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H44">
         <v>12</v>
       </c>
       <c r="I44">
-        <v>1.6191000000000001E-2</v>
+        <v>1.0219999999999999E-3</v>
       </c>
       <c r="J44">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="5"/>
+        <v>3413.8943248532291</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="6"/>
+        <v>9.7671232876712342</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="N44">
         <f t="shared" si="4"/>
-        <v>216.66357853128281</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="3"/>
         <v>1.0909089917355463</v>
       </c>
     </row>
-    <row r="45" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F45">
         <v>1000000</v>
       </c>
       <c r="G45">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H45">
         <v>13</v>
       </c>
       <c r="I45">
-        <v>1.6803999999999999E-2</v>
+        <v>9.5600000000000004E-4</v>
       </c>
       <c r="J45">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="5"/>
+        <v>3649.5815899581589</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="6"/>
+        <v>10.441422594142258</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="3"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="N45">
         <f t="shared" si="4"/>
-        <v>208.7598190906927</v>
-      </c>
-      <c r="K45">
-        <f t="shared" si="2"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="3"/>
         <v>1.0833332430555631</v>
       </c>
     </row>
-    <row r="46" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F46">
         <v>1000000</v>
       </c>
       <c r="G46">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H46">
         <v>14</v>
       </c>
       <c r="I46">
-        <v>1.7451999999999999E-2</v>
+        <v>8.8900000000000003E-4</v>
       </c>
       <c r="J46">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="5"/>
+        <v>3924.6344206974127</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="6"/>
+        <v>11.228346456692913</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="3"/>
+        <v>7.1428571428571438E-2</v>
+      </c>
+      <c r="N46">
         <f t="shared" si="4"/>
-        <v>201.00848040339218</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="2"/>
-        <v>7.1428571428571438E-2</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="3"/>
         <v>1.0769229940828466</v>
       </c>
     </row>
-    <row r="47" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F47">
         <v>1000000</v>
       </c>
       <c r="G47">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H47">
         <v>15</v>
       </c>
       <c r="I47">
-        <v>1.8022E-2</v>
+        <v>8.3299999999999997E-4</v>
       </c>
       <c r="J47">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="5"/>
+        <v>4188.4753901560625</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="6"/>
+        <v>11.983193277310924</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="3"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="N47">
         <f t="shared" si="4"/>
-        <v>194.65098213294863</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="2"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="3"/>
         <v>1.0714284948979647</v>
       </c>
     </row>
-    <row r="48" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F48">
         <v>1000000</v>
       </c>
       <c r="G48">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H48">
         <v>16</v>
       </c>
       <c r="I48">
-        <v>1.8637999999999998E-2</v>
+        <v>8.2399999999999997E-4</v>
       </c>
       <c r="J48">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="5"/>
+        <v>4234.2233009708734</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="6"/>
+        <v>12.114077669902912</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="3"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="N48">
         <f t="shared" si="4"/>
-        <v>188.21761991630004</v>
-      </c>
-      <c r="K48">
-        <f t="shared" si="2"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="3"/>
         <v>1.0666665955555603</v>
       </c>
     </row>
-    <row r="49" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F49">
         <v>1000000</v>
       </c>
       <c r="G49">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H49">
         <v>17</v>
       </c>
       <c r="I49">
-        <v>1.9231000000000002E-2</v>
+        <v>7.27E-4</v>
       </c>
       <c r="J49">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="5"/>
+        <v>4799.1746905089403</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="6"/>
+        <v>13.730398899587344</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="3"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="N49">
         <f t="shared" si="4"/>
-        <v>182.41381103426758</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="2"/>
-        <v>5.8823529411764705E-2</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="3"/>
         <v>1.0624999335937542</v>
       </c>
     </row>
-    <row r="50" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F50">
         <v>1000000</v>
       </c>
       <c r="G50">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H50">
         <v>18</v>
       </c>
       <c r="I50">
-        <v>1.9769999999999999E-2</v>
+        <v>6.8499999999999995E-4</v>
       </c>
       <c r="J50">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="5"/>
+        <v>5093.4306569343071</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="6"/>
+        <v>14.572262773722628</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="3"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="N50">
         <f t="shared" si="4"/>
-        <v>177.44056651492161</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="2"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="3"/>
         <v>1.0588234671280312</v>
       </c>
     </row>
-    <row r="51" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F51">
         <v>1000000</v>
       </c>
       <c r="G51">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H51">
         <v>19</v>
       </c>
       <c r="I51">
-        <v>2.0338999999999999E-2</v>
+        <v>7.1000000000000002E-4</v>
       </c>
       <c r="J51">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="5"/>
+        <v>4914.0845070422529</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="6"/>
+        <v>14.059154929577463</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="3"/>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="N51">
         <f t="shared" si="4"/>
-        <v>172.47652293623088</v>
-      </c>
-      <c r="K51">
-        <f t="shared" si="2"/>
-        <v>5.2631578947368418E-2</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="3"/>
         <v>1.0555554969135834</v>
       </c>
     </row>
-    <row r="52" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F52">
         <v>1000000</v>
       </c>
       <c r="G52">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H52">
         <v>20</v>
       </c>
       <c r="I52">
-        <v>2.0763E-2</v>
+        <v>6.7299999999999999E-4</v>
       </c>
       <c r="J52">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="5"/>
+        <v>5184.2496285289744</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="6"/>
+        <v>14.832095096582465</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="N52">
         <f t="shared" si="4"/>
-        <v>168.95439002070992</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="2"/>
-        <v>0.05</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="3"/>
         <v>1.0526315235457093</v>
       </c>
     </row>
-    <row r="53" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F53">
         <v>1000000</v>
       </c>
       <c r="G53">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H53">
         <v>21</v>
       </c>
       <c r="I53">
-        <v>2.1249000000000001E-2</v>
+        <v>6.4499999999999996E-4</v>
       </c>
       <c r="J53">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="5"/>
+        <v>5409.302325581396</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="6"/>
+        <v>15.475968992248063</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="3"/>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="N53">
         <f t="shared" si="4"/>
-        <v>165.09012188808885</v>
-      </c>
-      <c r="K53">
-        <f t="shared" si="2"/>
-        <v>4.7619047619047616E-2</v>
-      </c>
-      <c r="L53">
-        <f t="shared" si="3"/>
         <v>1.0499999475000028</v>
       </c>
     </row>
-    <row r="54" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F54">
         <v>1000000</v>
       </c>
       <c r="G54">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H54">
         <v>22</v>
       </c>
       <c r="I54">
-        <v>2.1651E-2</v>
+        <v>5.62E-4</v>
       </c>
       <c r="J54">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="5"/>
+        <v>6208.1850533807828</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="6"/>
+        <v>17.761565836298931</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="3"/>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="N54">
         <f t="shared" si="4"/>
-        <v>162.02484873677889</v>
-      </c>
-      <c r="K54">
-        <f t="shared" si="2"/>
-        <v>4.5454545454545456E-2</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="3"/>
         <v>1.0476189977324286</v>
       </c>
     </row>
-    <row r="55" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F55">
         <v>1000000</v>
       </c>
       <c r="G55">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H55">
         <v>23</v>
       </c>
       <c r="I55">
-        <v>2.2155999999999999E-2</v>
+        <v>5.8900000000000001E-4</v>
       </c>
       <c r="J55">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="5"/>
+        <v>5923.5993208828522</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="6"/>
+        <v>16.94736842105263</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="3"/>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="N55">
         <f t="shared" si="4"/>
-        <v>158.33182884997294</v>
-      </c>
-      <c r="K55">
-        <f t="shared" si="2"/>
-        <v>4.3478260869565216E-2</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="3"/>
         <v>1.0454544979338865</v>
       </c>
     </row>
-    <row r="56" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F56">
         <v>1000000</v>
       </c>
       <c r="G56">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H56">
         <v>24</v>
       </c>
       <c r="I56">
-        <v>2.2623000000000001E-2</v>
+        <v>5.2800000000000004E-4</v>
       </c>
       <c r="J56">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="5"/>
+        <v>6607.954545454545</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="6"/>
+        <v>18.905303030303028</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="3"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="N56">
         <f t="shared" si="4"/>
-        <v>155.06343102152675</v>
-      </c>
-      <c r="K56">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="3"/>
         <v>1.0434782155009472</v>
       </c>
     </row>
-    <row r="57" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F57">
         <v>1000000</v>
       </c>
       <c r="G57">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H57">
         <v>25</v>
       </c>
       <c r="I57">
-        <v>2.3146E-2</v>
+        <v>5.5800000000000001E-4</v>
       </c>
       <c r="J57">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="5"/>
+        <v>6252.6881720430101</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="6"/>
+        <v>17.888888888888889</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="N57">
         <f t="shared" si="4"/>
-        <v>151.55966473688758</v>
-      </c>
-      <c r="K57">
-        <f t="shared" si="2"/>
-        <v>0.04</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="3"/>
         <v>1.0416666232638907</v>
       </c>
     </row>
-    <row r="58" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F58">
         <v>1000000</v>
       </c>
       <c r="G58">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H58">
         <v>26</v>
       </c>
       <c r="I58">
-        <v>2.3569E-2</v>
+        <v>4.7899999999999999E-4</v>
       </c>
       <c r="J58">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="5"/>
+        <v>7283.9248434237998</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="6"/>
+        <v>20.839248434237994</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="3"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="N58">
         <f t="shared" si="4"/>
-        <v>148.83957741100599</v>
-      </c>
-      <c r="K58">
-        <f t="shared" si="2"/>
-        <v>3.8461538461538464E-2</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="3"/>
         <v>1.0399999584000015</v>
       </c>
     </row>
-    <row r="59" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F59">
         <v>1000000</v>
       </c>
       <c r="G59">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H59">
         <v>27</v>
       </c>
       <c r="I59">
-        <v>2.5309999999999999E-2</v>
+        <v>5.3399999999999997E-4</v>
       </c>
       <c r="J59">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="5"/>
+        <v>6533.7078651685397</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="6"/>
+        <v>18.692883895131086</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="3"/>
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="N59">
         <f t="shared" si="4"/>
-        <v>138.60134334255235</v>
-      </c>
-      <c r="K59">
-        <f t="shared" si="2"/>
-        <v>3.7037037037037035E-2</v>
-      </c>
-      <c r="L59">
-        <f t="shared" si="3"/>
         <v>1.0384614985207117</v>
       </c>
     </row>
-    <row r="60" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <f>I33/I60</f>
+        <v>19.49609375</v>
+      </c>
       <c r="F60">
         <v>1000000</v>
       </c>
       <c r="G60">
-        <v>3.508</v>
+        <v>3.4889999999999999</v>
       </c>
       <c r="H60">
         <v>28</v>
       </c>
       <c r="I60">
-        <v>5.2970999999999997E-2</v>
+        <v>5.1199999999999998E-4</v>
       </c>
       <c r="J60">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="5"/>
+        <v>6814.453125</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="6"/>
+        <v>19.49609375</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="3"/>
+        <v>3.5714285714285719E-2</v>
+      </c>
+      <c r="N60">
         <f t="shared" si="4"/>
-        <v>66.224915519812726</v>
-      </c>
-      <c r="K60">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285719E-2</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="3"/>
         <v>1.0370369986282593</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B25:D30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>